<commit_message>
added should_detect and naming of conditions in if
</commit_message>
<xml_diff>
--- a/src/raw_data/user_error_config.xlsx
+++ b/src/raw_data/user_error_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjasagrabnar/Desktop/magistrska/customer_data_cleanup/src/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ABD760-68BD-A443-B37F-076C0847A825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB47C7A-A2E8-074E-AAB6-195760E7925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="1020" windowWidth="16840" windowHeight="21080" xr2:uid="{626C9B5B-E040-FC44-A9E5-5F14A96B8943}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="127">
   <si>
     <t>error_code</t>
   </si>
@@ -414,6 +414,9 @@
   </si>
   <si>
     <t>validate</t>
+  </si>
+  <si>
+    <t>error_level</t>
   </si>
 </sst>
 </file>
@@ -797,1630 +800,1703 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCECA078-69AF-BC4B-BFC0-9E083A89901D}">
-  <dimension ref="A1:G70"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>125</v>
       </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1101</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>56</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1102</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
       <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1103</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>58</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1104</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>59</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1105</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
       <c r="F6" t="b">
         <v>1</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1106</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" t="b">
-        <v>1</v>
-      </c>
       <c r="F7" t="b">
         <v>1</v>
       </c>
-      <c r="G7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1107</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>62</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="b">
-        <v>1</v>
-      </c>
       <c r="F8" t="b">
         <v>1</v>
       </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1108</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>63</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="b">
-        <v>1</v>
-      </c>
       <c r="F9" t="b">
         <v>1</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1201</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>64</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" t="b">
-        <v>1</v>
-      </c>
       <c r="F10" t="b">
         <v>1</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1202</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" t="b">
-        <v>1</v>
-      </c>
       <c r="F11" t="b">
         <v>1</v>
       </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G11" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1203</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" t="b">
-        <v>1</v>
-      </c>
       <c r="F12" t="b">
         <v>1</v>
       </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1204</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>67</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>5</v>
       </c>
-      <c r="E13" t="b">
-        <v>1</v>
-      </c>
       <c r="F13" t="b">
         <v>1</v>
       </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G13" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1205</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="E14" t="b">
-        <v>1</v>
-      </c>
       <c r="F14" t="b">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" t="b">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>69</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>5</v>
       </c>
-      <c r="E15" t="b">
-        <v>1</v>
-      </c>
       <c r="F15" t="b">
         <v>1</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" t="b">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>2101</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="E16" t="b">
-        <v>1</v>
-      </c>
       <c r="F16" t="b">
         <v>1</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>2102</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>71</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>8</v>
       </c>
-      <c r="E17" t="b">
-        <v>1</v>
-      </c>
       <c r="F17" t="b">
         <v>1</v>
       </c>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G17" t="b">
+        <v>1</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2103</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1"/>
+      <c r="C18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>72</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>8</v>
       </c>
-      <c r="E18" t="b">
-        <v>1</v>
-      </c>
       <c r="F18" t="b">
         <v>1</v>
       </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>2104</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>73</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" t="b">
-        <v>1</v>
-      </c>
       <c r="F19" t="b">
         <v>1</v>
       </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G19" t="b">
+        <v>1</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>2105</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1"/>
+      <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>74</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="E20" t="b">
-        <v>1</v>
-      </c>
       <c r="F20" t="b">
         <v>1</v>
       </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G20" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>2106</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>8</v>
       </c>
-      <c r="E21" t="b">
-        <v>1</v>
-      </c>
       <c r="F21" t="b">
         <v>1</v>
       </c>
-      <c r="G21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>3101</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>76</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>8</v>
       </c>
-      <c r="E22" t="b">
-        <v>1</v>
-      </c>
       <c r="F22" t="b">
         <v>1</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>3102</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1"/>
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>77</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>8</v>
       </c>
-      <c r="E23" t="b">
-        <v>1</v>
-      </c>
       <c r="F23" t="b">
         <v>1</v>
       </c>
-      <c r="G23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>3103</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>78</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>8</v>
       </c>
-      <c r="E24" t="b">
-        <v>1</v>
-      </c>
       <c r="F24" t="b">
         <v>1</v>
       </c>
-      <c r="G24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3104</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1"/>
+      <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>79</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>8</v>
       </c>
-      <c r="E25" t="b">
-        <v>1</v>
-      </c>
       <c r="F25" t="b">
         <v>1</v>
       </c>
-      <c r="G25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>3105</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1"/>
+      <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
         <v>80</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="b">
-        <v>1</v>
-      </c>
       <c r="F26" t="b">
         <v>1</v>
       </c>
-      <c r="G26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>3106</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1"/>
+      <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>81</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>8</v>
       </c>
-      <c r="E27" t="b">
-        <v>1</v>
-      </c>
       <c r="F27" t="b">
         <v>1</v>
       </c>
-      <c r="G27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>3107</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1"/>
+      <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>82</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>8</v>
       </c>
-      <c r="E28" t="b">
-        <v>1</v>
-      </c>
       <c r="F28" t="b">
         <v>1</v>
       </c>
-      <c r="G28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>3108</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="1"/>
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>8</v>
       </c>
-      <c r="E29" t="b">
-        <v>1</v>
-      </c>
       <c r="F29" t="b">
         <v>1</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4101</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1"/>
+      <c r="C30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>84</v>
       </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="b">
-        <v>1</v>
+      <c r="E30" t="s">
+        <v>7</v>
       </c>
       <c r="F30" t="b">
         <v>1</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>4102</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="b">
-        <v>1</v>
+      <c r="E31" t="s">
+        <v>7</v>
       </c>
       <c r="F31" t="b">
         <v>1</v>
       </c>
-      <c r="G31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>4103</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1"/>
+      <c r="C32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>86</v>
       </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="b">
-        <v>1</v>
+      <c r="E32" t="s">
+        <v>7</v>
       </c>
       <c r="F32" t="b">
         <v>1</v>
       </c>
-      <c r="G32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>4104</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="1"/>
+      <c r="C33" t="s">
         <v>17</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>87</v>
       </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="b">
-        <v>1</v>
+      <c r="E33" t="s">
+        <v>7</v>
       </c>
       <c r="F33" t="b">
         <v>1</v>
       </c>
-      <c r="G33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G33" t="b">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>4105</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>88</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="b">
-        <v>1</v>
+      <c r="E34" t="s">
+        <v>7</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
       </c>
-      <c r="G34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G34" t="b">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>4106</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>89</v>
       </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="b">
-        <v>1</v>
+      <c r="E35" t="s">
+        <v>7</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
       </c>
-      <c r="G35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G35" t="b">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>4107</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="1"/>
+      <c r="C36" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
         <v>90</v>
       </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" t="b">
-        <v>1</v>
+      <c r="E36" t="s">
+        <v>7</v>
       </c>
       <c r="F36" t="b">
         <v>1</v>
       </c>
-      <c r="G36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G36" t="b">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>4108</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1"/>
+      <c r="C37" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>91</v>
       </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-      <c r="E37" t="b">
-        <v>1</v>
+      <c r="E37" t="s">
+        <v>7</v>
       </c>
       <c r="F37" t="b">
         <v>1</v>
       </c>
-      <c r="G37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G37" t="b">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>4109</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>92</v>
       </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" t="b">
-        <v>1</v>
+      <c r="E38" t="s">
+        <v>7</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
       </c>
-      <c r="G38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G38" t="b">
+        <v>1</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>4110</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1"/>
+      <c r="C39" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>93</v>
       </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-      <c r="E39" t="b">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>7</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G39" t="b">
+        <v>1</v>
+      </c>
+      <c r="H39" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>4111</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1"/>
+      <c r="C40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>94</v>
       </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="E40" t="b">
-        <v>1</v>
+      <c r="E40" t="s">
+        <v>7</v>
       </c>
       <c r="F40" t="b">
         <v>1</v>
       </c>
-      <c r="G40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G40" t="b">
+        <v>1</v>
+      </c>
+      <c r="H40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>4112</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>95</v>
       </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="b">
-        <v>1</v>
+      <c r="E41" t="s">
+        <v>7</v>
       </c>
       <c r="F41" t="b">
         <v>1</v>
       </c>
-      <c r="G41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G41" t="b">
+        <v>1</v>
+      </c>
+      <c r="H41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>4113</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" t="s">
         <v>36</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>96</v>
       </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" t="b">
-        <v>1</v>
+      <c r="E42" t="s">
+        <v>7</v>
       </c>
       <c r="F42" t="b">
         <v>1</v>
       </c>
-      <c r="G42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" t="b">
+        <v>1</v>
+      </c>
+      <c r="H42" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>4114</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="1"/>
+      <c r="C43" t="s">
         <v>21</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>97</v>
       </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="E43" t="b">
-        <v>1</v>
+      <c r="E43" t="s">
+        <v>7</v>
       </c>
       <c r="F43" t="b">
         <v>1</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G43" t="b">
+        <v>1</v>
+      </c>
+      <c r="H43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>4201</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1"/>
+      <c r="C44" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>98</v>
       </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="E44" t="b">
-        <v>1</v>
+      <c r="E44" t="s">
+        <v>7</v>
       </c>
       <c r="F44" t="b">
         <v>1</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G44" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>4202</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1"/>
+      <c r="C45" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>99</v>
       </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="E45" t="b">
-        <v>1</v>
+      <c r="E45" t="s">
+        <v>7</v>
       </c>
       <c r="F45" t="b">
         <v>1</v>
       </c>
-      <c r="G45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>4203</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1"/>
+      <c r="C46" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>100</v>
       </c>
-      <c r="D46" t="s">
-        <v>7</v>
-      </c>
-      <c r="E46" t="b">
-        <v>1</v>
+      <c r="E46" t="s">
+        <v>7</v>
       </c>
       <c r="F46" t="b">
         <v>1</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G46" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>4204</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1"/>
+      <c r="C47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>101</v>
       </c>
-      <c r="D47" t="s">
-        <v>7</v>
-      </c>
-      <c r="E47" t="b">
-        <v>1</v>
+      <c r="E47" t="s">
+        <v>7</v>
       </c>
       <c r="F47" t="b">
         <v>1</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G47" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>4205</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1"/>
+      <c r="C48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>102</v>
       </c>
-      <c r="D48" t="s">
-        <v>7</v>
-      </c>
-      <c r="E48" t="b">
-        <v>1</v>
+      <c r="E48" t="s">
+        <v>7</v>
       </c>
       <c r="F48" t="b">
         <v>1</v>
       </c>
-      <c r="G48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G48" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>4206</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1"/>
+      <c r="C49" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>103</v>
       </c>
-      <c r="D49" t="s">
-        <v>7</v>
-      </c>
-      <c r="E49" t="b">
-        <v>1</v>
+      <c r="E49" t="s">
+        <v>7</v>
       </c>
       <c r="F49" t="b">
         <v>1</v>
       </c>
-      <c r="G49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G49" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>4207</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1"/>
+      <c r="C50" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>104</v>
       </c>
-      <c r="D50" t="s">
-        <v>7</v>
-      </c>
-      <c r="E50" t="b">
-        <v>1</v>
+      <c r="E50" t="s">
+        <v>7</v>
       </c>
       <c r="F50" t="b">
         <v>1</v>
       </c>
-      <c r="G50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G50" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>4208</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1"/>
+      <c r="C51" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>105</v>
       </c>
-      <c r="D51" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" t="b">
-        <v>1</v>
+      <c r="E51" t="s">
+        <v>7</v>
       </c>
       <c r="F51" t="b">
         <v>1</v>
       </c>
-      <c r="G51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>4209</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="1"/>
+      <c r="C52" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>106</v>
       </c>
-      <c r="D52" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" t="b">
-        <v>1</v>
+      <c r="E52" t="s">
+        <v>7</v>
       </c>
       <c r="F52" t="b">
         <v>1</v>
       </c>
-      <c r="G52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>4210</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="1"/>
+      <c r="C53" t="s">
         <v>44</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>107</v>
       </c>
-      <c r="D53" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" t="b">
-        <v>1</v>
+      <c r="E53" t="s">
+        <v>7</v>
       </c>
       <c r="F53" t="b">
         <v>1</v>
       </c>
-      <c r="G53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>4211</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="1"/>
+      <c r="C54" t="s">
         <v>45</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>108</v>
       </c>
-      <c r="D54" t="s">
-        <v>7</v>
-      </c>
-      <c r="E54" t="b">
-        <v>1</v>
+      <c r="E54" t="s">
+        <v>7</v>
       </c>
       <c r="F54" t="b">
         <v>1</v>
       </c>
-      <c r="G54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>4212</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1"/>
+      <c r="C55" t="s">
         <v>46</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
         <v>109</v>
       </c>
-      <c r="D55" t="s">
-        <v>7</v>
-      </c>
-      <c r="E55" t="b">
-        <v>1</v>
+      <c r="E55" t="s">
+        <v>7</v>
       </c>
       <c r="F55" t="b">
         <v>1</v>
       </c>
-      <c r="G55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>4301</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1"/>
+      <c r="C56" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>110</v>
       </c>
-      <c r="D56" t="s">
-        <v>7</v>
-      </c>
-      <c r="E56" t="b">
-        <v>1</v>
+      <c r="E56" t="s">
+        <v>7</v>
       </c>
       <c r="F56" t="b">
         <v>1</v>
       </c>
-      <c r="G56" t="s">
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>4302</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1"/>
+      <c r="C57" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
         <v>111</v>
       </c>
-      <c r="D57" t="s">
-        <v>7</v>
-      </c>
-      <c r="E57" t="b">
-        <v>1</v>
+      <c r="E57" t="s">
+        <v>7</v>
       </c>
       <c r="F57" t="b">
         <v>1</v>
       </c>
-      <c r="G57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>4303</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1"/>
+      <c r="C58" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C58" t="s">
+      <c r="D58" t="s">
         <v>112</v>
       </c>
-      <c r="D58" t="s">
-        <v>7</v>
-      </c>
-      <c r="E58" t="b">
-        <v>1</v>
+      <c r="E58" t="s">
+        <v>7</v>
       </c>
       <c r="F58" t="b">
         <v>1</v>
       </c>
-      <c r="G58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>4304</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1"/>
+      <c r="C59" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C59" t="s">
+      <c r="D59" t="s">
         <v>113</v>
       </c>
-      <c r="D59" t="s">
-        <v>7</v>
-      </c>
-      <c r="E59" t="b">
-        <v>1</v>
+      <c r="E59" t="s">
+        <v>7</v>
       </c>
       <c r="F59" t="b">
         <v>1</v>
       </c>
-      <c r="G59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>4305</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1"/>
+      <c r="C60" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>114</v>
       </c>
-      <c r="D60" t="s">
-        <v>7</v>
-      </c>
-      <c r="E60" t="b">
-        <v>1</v>
+      <c r="E60" t="s">
+        <v>7</v>
       </c>
       <c r="F60" t="b">
         <v>1</v>
       </c>
-      <c r="G60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>4306</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1"/>
+      <c r="C61" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>115</v>
       </c>
-      <c r="D61" t="s">
-        <v>7</v>
-      </c>
-      <c r="E61" t="b">
-        <v>1</v>
+      <c r="E61" t="s">
+        <v>7</v>
       </c>
       <c r="F61" t="b">
         <v>1</v>
       </c>
-      <c r="G61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G61" t="b">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>4307</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1"/>
+      <c r="C62" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>116</v>
       </c>
-      <c r="D62" t="s">
-        <v>7</v>
-      </c>
-      <c r="E62" t="b">
-        <v>1</v>
+      <c r="E62" t="s">
+        <v>7</v>
       </c>
       <c r="F62" t="b">
         <v>1</v>
       </c>
-      <c r="G62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G62" t="b">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>4401</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1"/>
+      <c r="C63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
         <v>117</v>
       </c>
-      <c r="D63" t="s">
-        <v>7</v>
-      </c>
-      <c r="E63" t="b">
-        <v>1</v>
+      <c r="E63" t="s">
+        <v>7</v>
       </c>
       <c r="F63" t="b">
         <v>1</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" t="b">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>4402</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1"/>
+      <c r="C64" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
         <v>118</v>
       </c>
-      <c r="D64" t="s">
-        <v>7</v>
-      </c>
-      <c r="E64" t="b">
-        <v>1</v>
+      <c r="E64" t="s">
+        <v>7</v>
       </c>
       <c r="F64" t="b">
         <v>1</v>
       </c>
-      <c r="G64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G64" t="b">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>4403</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="1"/>
+      <c r="C65" t="s">
         <v>24</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>119</v>
       </c>
-      <c r="D65" t="s">
-        <v>7</v>
-      </c>
-      <c r="E65" t="b">
-        <v>1</v>
+      <c r="E65" t="s">
+        <v>7</v>
       </c>
       <c r="F65" t="b">
         <v>1</v>
       </c>
-      <c r="G65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G65" t="b">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>4404</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1"/>
+      <c r="C66" t="s">
         <v>17</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>120</v>
       </c>
-      <c r="D66" t="s">
-        <v>7</v>
-      </c>
-      <c r="E66" t="b">
-        <v>1</v>
+      <c r="E66" t="s">
+        <v>7</v>
       </c>
       <c r="F66" t="b">
         <v>1</v>
       </c>
-      <c r="G66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G66" t="b">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>4405</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="1"/>
+      <c r="C67" t="s">
         <v>52</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>121</v>
       </c>
-      <c r="D67" t="s">
-        <v>7</v>
-      </c>
-      <c r="E67" t="b">
-        <v>1</v>
+      <c r="E67" t="s">
+        <v>7</v>
       </c>
       <c r="F67" t="b">
         <v>1</v>
       </c>
-      <c r="G67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G67" t="b">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>4406</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="1"/>
+      <c r="C68" t="s">
         <v>31</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>122</v>
       </c>
-      <c r="D68" t="s">
-        <v>7</v>
-      </c>
-      <c r="E68" t="b">
-        <v>1</v>
+      <c r="E68" t="s">
+        <v>7</v>
       </c>
       <c r="F68" t="b">
         <v>1</v>
       </c>
-      <c r="G68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G68" t="b">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>4407</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="1"/>
+      <c r="C69" t="s">
         <v>18</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>123</v>
       </c>
-      <c r="D69" t="s">
-        <v>7</v>
-      </c>
-      <c r="E69" t="b">
-        <v>1</v>
+      <c r="E69" t="s">
+        <v>7</v>
       </c>
       <c r="F69" t="b">
         <v>1</v>
       </c>
-      <c r="G69" t="s">
+      <c r="G69" t="b">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="1"/>
+      <c r="C70" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
         <v>124</v>
       </c>
-      <c r="D70" t="s">
-        <v>7</v>
-      </c>
-      <c r="E70" t="b">
-        <v>1</v>
+      <c r="E70" t="s">
+        <v>7</v>
       </c>
       <c r="F70" t="b">
         <v>1</v>
       </c>
-      <c r="G70" t="s">
+      <c r="G70" t="b">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correction of phone errors
</commit_message>
<xml_diff>
--- a/src/raw_data/user_error_config.xlsx
+++ b/src/raw_data/user_error_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tjasagrabnar/Desktop/magistrska/customer_data_cleanup/src/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5608A4-DDD6-B844-9C98-79DD2466AF54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE8AD964-5C95-A745-89E7-2F0AE3F78B40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23020" yWindow="1020" windowWidth="11040" windowHeight="21080" xr2:uid="{626C9B5B-E040-FC44-A9E5-5F14A96B8943}"/>
   </bookViews>
@@ -494,7 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -502,6 +501,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCECA078-69AF-BC4B-BFC0-9E083A89901D}">
   <dimension ref="A1:G69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="169" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -877,10 +879,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+      <c r="A2" s="12">
         <v>1101</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
@@ -900,10 +902,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
+      <c r="A3" s="12">
         <v>1102</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="C3" t="s">
@@ -923,10 +925,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+      <c r="A4" s="12">
         <v>1103</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="15" t="s">
         <v>14</v>
       </c>
       <c r="C4" t="s">
@@ -946,10 +948,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8">
+      <c r="A5" s="12">
         <v>1104</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
@@ -969,10 +971,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
+      <c r="A6" s="12">
         <v>1105</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C6" t="s">
@@ -992,10 +994,10 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
+      <c r="A7" s="12">
         <v>1106</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C7" t="s">
@@ -1015,10 +1017,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
+      <c r="A8" s="12">
         <v>1107</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
@@ -1153,10 +1155,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="15">
+      <c r="A14" s="14">
         <v>2101</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
@@ -1176,10 +1178,10 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="15">
+      <c r="A15" s="14">
         <v>2102</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
@@ -1199,10 +1201,10 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="15">
+      <c r="A16" s="14">
         <v>2103</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
@@ -1222,10 +1224,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="15">
+      <c r="A17" s="14">
         <v>2104</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
@@ -1245,10 +1247,10 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="15">
+      <c r="A18" s="14">
         <v>2105</v>
       </c>
-      <c r="B18" s="11" t="s">
+      <c r="B18" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C18" t="s">
@@ -1268,10 +1270,10 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="15">
+      <c r="A19" s="14">
         <v>2106</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="10" t="s">
         <v>125</v>
       </c>
       <c r="C19" t="s">
@@ -1291,10 +1293,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>123</v>
       </c>
       <c r="C20" t="s">
@@ -1314,10 +1316,10 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="10" t="s">
         <v>127</v>
       </c>
       <c r="C21" t="s">
@@ -1325,10 +1327,10 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
+      <c r="A22" s="8">
         <v>3101</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C22" t="s">
@@ -1348,10 +1350,10 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
+      <c r="A23" s="8">
         <v>3102</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
@@ -1371,10 +1373,10 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
+      <c r="A24" s="8">
         <v>3103</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>21</v>
       </c>
       <c r="C24" t="s">
@@ -1394,10 +1396,10 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
+      <c r="A25" s="8">
         <v>3104</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C25" t="s">
@@ -1417,10 +1419,10 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
+      <c r="A26" s="8">
         <v>3105</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C26" t="s">
@@ -1440,10 +1442,10 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
+      <c r="A27" s="8">
         <v>3106</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C27" t="s">
@@ -1463,10 +1465,10 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
+      <c r="A28" s="8">
         <v>3107</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="9" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
@@ -1486,10 +1488,10 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
+      <c r="A29" s="8">
         <v>3108</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C29" t="s">
@@ -1509,10 +1511,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>4101</v>
       </c>
-      <c r="B30" s="11" t="s">
+      <c r="B30" s="10" t="s">
         <v>12</v>
       </c>
       <c r="C30" t="s">
@@ -1532,10 +1534,10 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="13">
+      <c r="A31" s="12">
         <v>4102</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C31" t="s">
@@ -1555,10 +1557,10 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="13">
+      <c r="A32" s="12">
         <v>4103</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C32" t="s">
@@ -1578,10 +1580,10 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="13">
+      <c r="A33" s="12">
         <v>4104</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C33" t="s">
@@ -1601,10 +1603,10 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+      <c r="A34" s="12">
         <v>4105</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C34" t="s">
@@ -1624,10 +1626,10 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="13">
+      <c r="A35" s="12">
         <v>4106</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C35" t="s">
@@ -1647,10 +1649,10 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="13">
+      <c r="A36" s="12">
         <v>4107</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>28</v>
       </c>
       <c r="C36" t="s">
@@ -1670,10 +1672,10 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="13">
+      <c r="A37" s="12">
         <v>4108</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>29</v>
       </c>
       <c r="C37" t="s">
@@ -1693,10 +1695,10 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="13">
+      <c r="A38" s="12">
         <v>4109</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C38" t="s">
@@ -1716,7 +1718,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>4110</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -1739,10 +1741,10 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="13">
+      <c r="A40" s="12">
         <v>4111</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C40" t="s">
@@ -1762,7 +1764,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>4112</v>
       </c>
       <c r="B41" s="9" t="s">
@@ -1785,10 +1787,10 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="13">
+      <c r="A42" s="12">
         <v>4113</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>33</v>
       </c>
       <c r="C42" t="s">

</xml_diff>